<commit_message>
rename last sheet 'Insert Values'
</commit_message>
<xml_diff>
--- a/DB Scripts/Components Detail.xlsx
+++ b/DB Scripts/Components Detail.xlsx
@@ -24,7 +24,7 @@
     <sheet name="ANNOUCEMENT" sheetId="13" r:id="rId10"/>
     <sheet name="PARAMETER" sheetId="14" r:id="rId11"/>
     <sheet name="Vaccine Combination" sheetId="2" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId13"/>
+    <sheet name="Insert Values" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -3318,7 +3318,7 @@
   <dimension ref="A2:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5595,6 +5595,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x010100A30F3884CD43244294355762AE14FDC0" ma:contentTypeVersion="13" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="d6abdbf5296efb927e779bc42333b79d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c8b53866-fdfd-416a-aee2-e50c3ae941dd" xmlns:ns4="9d433cf1-fba1-428a-9634-baf48b90bf9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cbc3d42f92fe2e49d2b946bcae330cb" ns3:_="" ns4:_="">
     <xsd:import namespace="c8b53866-fdfd-416a-aee2-e50c3ae941dd"/>
@@ -5817,15 +5826,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5833,6 +5833,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEDA33A1-F718-434B-8088-40E4E15F457F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7B083-9D0F-4795-94A6-C1128A2A5DD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5847,14 +5855,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEDA33A1-F718-434B-8088-40E4E15F457F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
draw class diagram update relationship table
</commit_message>
<xml_diff>
--- a/DB Scripts/Components Detail.xlsx
+++ b/DB Scripts/Components Detail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="729" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="ACCOUNT" sheetId="10" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="HEALTH" sheetId="9" r:id="rId9"/>
     <sheet name="ANNOUCEMENT" sheetId="13" r:id="rId10"/>
     <sheet name="PARAMETER" sheetId="14" r:id="rId11"/>
-    <sheet name="Vaccine Combination" sheetId="2" r:id="rId12"/>
-    <sheet name="Insert Values" sheetId="15" r:id="rId13"/>
+    <sheet name="STATISTIC" sheetId="17" r:id="rId12"/>
+    <sheet name="Vaccine Combination" sheetId="2" r:id="rId13"/>
+    <sheet name="Insert Values" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +42,7 @@
     <author>operator</author>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0">
+    <comment ref="E12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -639,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="248">
   <si>
     <t>PERSON</t>
   </si>
@@ -1372,6 +1373,18 @@
   </si>
   <si>
     <t>nttnntt</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>THONG KE MUI CO BAN</t>
+  </si>
+  <si>
+    <t>STATISTIC</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -1925,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,75 +1991,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>187</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>188</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2062,12 +2083,12 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2194,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,6 +2345,46 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3">
+        <v>170000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:B22"/>
   <sheetViews>
@@ -2394,7 +2455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
@@ -3297,8 +3358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3679,7 +3740,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,8 +4609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4907,18 +4968,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4941,14 +5002,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEDA33A1-F718-434B-8088-40E4E15F457F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0203D343-F538-49C2-AACC-F77D433EB844}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4963,4 +5016,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEDA33A1-F718-434B-8088-40E4E15F457F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Query log, some table.sql file
</commit_message>
<xml_diff>
--- a/DB Scripts/Components Detail.xlsx
+++ b/DB Scripts/Components Detail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="729" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="ACCOUNT" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>operator</author>
   </authors>
   <commentList>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -640,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="291">
   <si>
     <t>PERSON</t>
   </si>
@@ -2067,10 +2067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,97 +2106,89 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>132</v>
       </c>
+      <c r="E9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="E12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2477,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -4529,8 +4521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5199,12 +5191,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x010100A30F3884CD43244294355762AE14FDC0" ma:contentTypeVersion="13" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="d6abdbf5296efb927e779bc42333b79d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c8b53866-fdfd-416a-aee2-e50c3ae941dd" xmlns:ns4="9d433cf1-fba1-428a-9634-baf48b90bf9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cbc3d42f92fe2e49d2b946bcae330cb" ns3:_="" ns4:_="">
     <xsd:import namespace="c8b53866-fdfd-416a-aee2-e50c3ae941dd"/>
@@ -5427,6 +5413,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5437,23 +5429,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0203D343-F538-49C2-AACC-F77D433EB844}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c8b53866-fdfd-416a-aee2-e50c3ae941dd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9d433cf1-fba1-428a-9634-baf48b90bf9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56A7B083-9D0F-4795-94A6-C1128A2A5DD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5472,6 +5447,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0203D343-F538-49C2-AACC-F77D433EB844}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c8b53866-fdfd-416a-aee2-e50c3ae941dd"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9d433cf1-fba1-428a-9634-baf48b90bf9f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEDA33A1-F718-434B-8088-40E4E15F457F}">
   <ds:schemaRefs>

</xml_diff>